<commit_message>
Download Yearly report Projects on acme website
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokul\Documents\UiPath\Download_YearlyReports\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F31CF5-9CFB-452C-AD7A-7C1CE11E82ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5859485E-0AF8-4464-BE50-EA799B71605C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -475,7 +475,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2067,7 +2066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -2381,7 +2380,7 @@
       <c r="A45" t="s">
         <v>125</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>